<commit_message>
Added notes to example
</commit_message>
<xml_diff>
--- a/examples/iris_gptable.xlsx
+++ b/examples/iris_gptable.xlsx
@@ -440,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -654,6 +654,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="9">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Separated methods for writing notes and annotations
</commit_message>
<xml_diff>
--- a/examples/iris_gptable.xlsx
+++ b/examples/iris_gptable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\gptables\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34DB179-F397-4DD3-8EE9-B5BE794A07A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D1911C-0EB0-4E79-AF0E-B411493D79F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="2745" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="1965" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iris flower dimensions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Iris(1) flower dimensions</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>(2: I've got 99 problems and taxonomy is one.)</t>
+  </si>
+  <si>
+    <t>(This note hath no reference.)</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -726,14 +731,19 @@
         <v>16</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ability to ref note in table headings and index
</commit_message>
<xml_diff>
--- a/examples/iris_gptable.xlsx
+++ b/examples/iris_gptable.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\gptables\examples\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D1911C-0EB0-4E79-AF0E-B411493D79F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1965" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="iris flower dimensions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Iris(1) flower dimensions</t>
   </si>
@@ -37,7 +31,7 @@
     <t>cm(2)</t>
   </si>
   <si>
-    <t>All</t>
+    <t>All(3)</t>
   </si>
   <si>
     <t>Setosa</t>
@@ -61,7 +55,7 @@
     <t>Petal Width</t>
   </si>
   <si>
-    <t>Sepal Length</t>
+    <t>Sepal Length(4)</t>
   </si>
   <si>
     <t>Sepal Width</t>
@@ -77,6 +71,12 @@
   </si>
   <si>
     <t>(2: I've got 99 problems and taxonomy is one.)</t>
+  </si>
+  <si>
+    <t>(3: All species of the Iris genus)</t>
+  </si>
+  <si>
+    <t>(4: Length of the largest sepal)</t>
   </si>
   <si>
     <t>(This note hath no reference.)</t>
@@ -85,8 +85,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,14 +173,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -227,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,27 +251,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,24 +285,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -504,31 +460,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -545,7 +499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6" t="s">
@@ -561,7 +515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -569,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="8">
-        <v>3.7586666666666662</v>
+        <v>3.758666666666666</v>
       </c>
       <c r="D7" s="8">
         <v>1.464</v>
@@ -578,10 +532,10 @@
         <v>4.26</v>
       </c>
       <c r="F7" s="8">
-        <v>5.5519999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5.552</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -589,19 +543,19 @@
         <v>11</v>
       </c>
       <c r="C8" s="8">
-        <v>4.3499999999999996</v>
+        <v>4.35</v>
       </c>
       <c r="D8" s="8">
         <v>1.5</v>
       </c>
       <c r="E8" s="8">
-        <v>4.3499999999999996</v>
+        <v>4.35</v>
       </c>
       <c r="F8" s="8">
         <v>5.55</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -612,16 +566,16 @@
         <v>1.198666666666667</v>
       </c>
       <c r="D9" s="8">
-        <v>0.24399999999999991</v>
+        <v>0.2439999999999999</v>
       </c>
       <c r="E9" s="8">
-        <v>1.3260000000000001</v>
+        <v>1.326</v>
       </c>
       <c r="F9" s="8">
-        <v>2.0259999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.026</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -641,7 +595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -649,19 +603,19 @@
         <v>10</v>
       </c>
       <c r="C11" s="8">
-        <v>5.8433333333333337</v>
+        <v>5.843333333333334</v>
       </c>
       <c r="D11" s="8">
-        <v>5.0059999999999993</v>
+        <v>5.005999999999999</v>
       </c>
       <c r="E11" s="8">
-        <v>5.9359999999999999</v>
+        <v>5.936</v>
       </c>
       <c r="F11" s="8">
-        <v>6.5879999999999983</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6.587999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -681,7 +635,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -689,7 +643,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="8">
-        <v>3.0539999999999998</v>
+        <v>3.054</v>
       </c>
       <c r="D13" s="8">
         <v>3.418000000000001</v>
@@ -698,10 +652,10 @@
         <v>2.77</v>
       </c>
       <c r="F13" s="8">
-        <v>2.9740000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.974</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -721,29 +675,39 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="9" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug to return pos
</commit_message>
<xml_diff>
--- a/examples/iris_gptable.xlsx
+++ b/examples/iris_gptable.xlsx
@@ -114,14 +114,14 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -159,12 +159,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -681,7 +681,7 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="9" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>